<commit_message>
Separate XMLParser in XMLManager
</commit_message>
<xml_diff>
--- a/ItShop/test.xlsx
+++ b/ItShop/test.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Sales Report" sheetId="1" r:id="Rd0d2920dd2574c99"/>
+    <sheet name="Sales Report" sheetId="1" r:id="R391a988b238f4a37"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Sales Report'!$1:$2,'Sales Report'!$A:$G,'Sales Report'!$1:$2</definedName>
@@ -112,11 +112,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.8765889485677" customWidth="1"/>
-    <col min="2" max="2" width="9.96565246582031" customWidth="1"/>
-    <col min="3" max="3" width="6.42502746582031" customWidth="1"/>
-    <col min="4" max="4" width="30.1160827636719" customWidth="1"/>
-    <col min="5" max="5" width="21.1088785807292" customWidth="1"/>
+    <col min="1" max="1" width="11.5381147596571" customWidth="1"/>
+    <col min="2" max="2" width="10.5892215304905" customWidth="1"/>
+    <col min="3" max="3" width="6.90107133653429" customWidth="1"/>
+    <col min="4" max="4" width="31.5792507595486" customWidth="1"/>
+    <col min="5" max="5" width="22.1967502170139" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
JSON import in MySQL database; Many bugs fixed
</commit_message>
<xml_diff>
--- a/ItShop/test.xlsx
+++ b/ItShop/test.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Sales Report" sheetId="1" r:id="R391a988b238f4a37"/>
+    <sheet name="Sales Report" sheetId="1" r:id="R867ec6089f454037"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Sales Report'!$1:$2,'Sales Report'!$A:$G,'Sales Report'!$1:$2</definedName>
@@ -14,27 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Store Name</t>
+    <t>Product Name</t>
   </si>
   <si>
-    <t>Total Sales</t>
+    <t>Category Name</t>
   </si>
   <si>
-    <t>Marge</t>
+    <t>From</t>
   </si>
   <si>
-    <t>Best Selling Product</t>
+    <t>To</t>
   </si>
   <si>
-    <t>Most profitable Product</t>
+    <t>Total Quantity Sold</t>
   </si>
   <si>
-    <t>Ninja</t>
+    <t>Ninja dildo</t>
   </si>
   <si>
-    <t>high-end gaming desctop computer</t>
+    <t>dildos</t>
+  </si>
+  <si>
+    <t>8/3/2014 12:00:00 AM</t>
+  </si>
+  <si>
+    <t>666</t>
   </si>
 </sst>
 </file>
@@ -112,11 +118,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5381147596571" customWidth="1"/>
-    <col min="2" max="2" width="10.5892215304905" customWidth="1"/>
-    <col min="3" max="3" width="6.90107133653429" customWidth="1"/>
-    <col min="4" max="4" width="31.5792507595486" customWidth="1"/>
-    <col min="5" max="5" width="22.1967502170139" customWidth="1"/>
+    <col min="1" max="1" width="14.2726287841797" customWidth="1"/>
+    <col min="2" max="2" width="15.243518284389" customWidth="1"/>
+    <col min="3" max="3" width="21.4289703369141" customWidth="1"/>
+    <col min="4" max="4" width="4.69366863795689" customWidth="1"/>
+    <col min="5" max="5" width="18.7372861589704" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -140,14 +146,14 @@
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0">
-        <v>12312</v>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
       </c>
-      <c r="C2" s="0">
-        <v>123</v>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -165,8 +171,8 @@
     </row>
   </sheetData>
   <headerFooter>
-    <oddHeader>&amp;C&amp;24&amp;U&amp;"Arial,Regular Bold" Sales Report</oddHeader>
-    <oddFooter>&amp;C&amp;A&amp;RPage &amp;P of &amp;N</oddFooter>
+    <oddHeader>&amp;R&amp;24&amp;U&amp;"Arial,Regular Bold" Sales Report</oddHeader>
+    <oddFooter>&amp;LPage &amp;P of &amp;N&amp;C&amp;A</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>